<commit_message>
Update & finish carowoners
</commit_message>
<xml_diff>
--- a/bdd/exosql/comprehension.xlsx
+++ b/bdd/exosql/comprehension.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rbounatirou\Documents\repos\CDA2210\bdd\exosql\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC37127D-83B4-48FC-A5A6-2DD18ECFFEE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA09765-6186-42B2-B7DB-3A13A2EF477F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{F190465E-BB19-47FE-9E4B-767B4F574E17}"/>
   </bookViews>
@@ -523,7 +523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DD07120-34EB-4824-8F68-EBE771115CBA}">
   <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>

</xml_diff>